<commit_message>
Adds KNN model saves
</commit_message>
<xml_diff>
--- a/Model Results Overview.xlsx
+++ b/Model Results Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df8978671778c259/Desktop/repos/Homework/Wine_Quality_Predictor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{C5952579-04A8-4BFA-A758-230286535F9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BBEF9B22-EA0F-456F-8ADB-10A143D58448}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{C5952579-04A8-4BFA-A758-230286535F9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EB5C5522-7E66-484D-ABA3-F37CC5BB0A94}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8A3C5073-7F06-4D4F-B578-7570066F7EA9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="51">
   <si>
     <t>Power transformer</t>
   </si>
@@ -184,6 +184,14 @@
   <si>
     <t>Top 5 features: Alcohol, volatile acidity, density, free sulfur dioxide, total sulfur dioxide
 Per GridSearch best params: 'criterion': 'gini', 'max_depth': 125, 'n_estimators': 50</t>
+  </si>
+  <si>
+    <t>Top Features: Alcohol, sulphates. Free sulfur dioxide, chlorides, volatile acidity, total sulfure dioxide
+Best Params: Best leaf_size: 1 Best p: 2 Best n_neighbors: 1</t>
+  </si>
+  <si>
+    <t>Top Features: All with Chlorides having the least weight
+Best Params: n_neighbors = 1, leaf_size = 1, p = 1</t>
   </si>
 </sst>
 </file>
@@ -425,11 +433,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -443,31 +459,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,1300 +824,1308 @@
   <sheetData>
     <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="7"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="17"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="3" t="s">
+      <c r="I3" s="19"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="3" t="s">
+      <c r="L3" s="19"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="3" t="s">
+      <c r="O3" s="19"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="3" t="s">
+      <c r="R3" s="19"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="10"/>
+      <c r="U3" s="23"/>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="9"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="9"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="L4" s="2"/>
-      <c r="M4" s="9"/>
+      <c r="M4" s="3"/>
       <c r="N4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="9"/>
+      <c r="P4" s="3"/>
       <c r="Q4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="R4" s="2"/>
-      <c r="S4" s="9"/>
+      <c r="S4" s="3"/>
       <c r="T4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="12"/>
+      <c r="U4" s="5"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="10">
         <v>0.13993900000000001</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="2">
         <v>0.14168600000000001</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="2">
         <v>0.14368</v>
       </c>
-      <c r="J5" s="9"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="L5" s="2">
         <v>0.142153</v>
       </c>
-      <c r="M5" s="9"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="O5" s="2">
         <v>0.138017</v>
       </c>
-      <c r="P5" s="9"/>
+      <c r="P5" s="3"/>
       <c r="Q5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="R5" s="2">
         <v>0.13892699999999999</v>
       </c>
-      <c r="S5" s="9"/>
+      <c r="S5" s="3"/>
       <c r="T5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="12">
+      <c r="U5" s="5">
         <v>0.14053299999999999</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="10">
         <v>0.11552800000000001</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="2">
         <v>0.115385</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="2">
         <v>0.114435</v>
       </c>
-      <c r="J6" s="9"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L6" s="2">
         <v>0.116024</v>
       </c>
-      <c r="M6" s="9"/>
+      <c r="M6" s="3"/>
       <c r="N6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="O6" s="2">
         <v>0.11354499999999999</v>
       </c>
-      <c r="P6" s="9"/>
+      <c r="P6" s="3"/>
       <c r="Q6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="R6" s="2">
         <v>0.11336400000000001</v>
       </c>
-      <c r="S6" s="9"/>
+      <c r="S6" s="3"/>
       <c r="T6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="12">
+      <c r="U6" s="5">
         <v>0.117383</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="10">
         <v>0.111919</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="2">
         <v>0.110288</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="2">
         <v>0.10578899999999999</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="2">
         <v>0.10800899999999999</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="O7" s="2">
         <v>0.11115700000000001</v>
       </c>
-      <c r="P7" s="9"/>
+      <c r="P7" s="3"/>
       <c r="Q7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="R7" s="2">
         <v>0.110942</v>
       </c>
-      <c r="S7" s="9"/>
+      <c r="S7" s="3"/>
       <c r="T7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="U7" s="12">
+      <c r="U7" s="5">
         <v>0.109418</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="10">
         <v>9.7774E-2</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="2">
         <v>9.5348000000000002E-2</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="2">
         <v>9.7652000000000003E-2</v>
       </c>
-      <c r="J8" s="9"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="L8" s="2">
         <v>9.8285999999999998E-2</v>
       </c>
-      <c r="M8" s="9"/>
+      <c r="M8" s="3"/>
       <c r="N8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="O8" s="2">
         <v>9.6140000000000003E-2</v>
       </c>
-      <c r="P8" s="9"/>
+      <c r="P8" s="3"/>
       <c r="Q8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="R8" s="2">
         <v>9.6393000000000006E-2</v>
       </c>
-      <c r="S8" s="9"/>
+      <c r="S8" s="3"/>
       <c r="T8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U8" s="12">
+      <c r="U8" s="5">
         <v>9.8334000000000005E-2</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="10">
         <v>8.4717000000000001E-2</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="2">
         <v>8.5607000000000003E-2</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="2">
         <v>8.4988999999999995E-2</v>
       </c>
-      <c r="J9" s="9"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L9" s="2">
         <v>8.5993E-2</v>
       </c>
-      <c r="M9" s="9"/>
+      <c r="M9" s="3"/>
       <c r="N9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="O9" s="2">
         <v>8.8612999999999997E-2</v>
       </c>
-      <c r="P9" s="9"/>
+      <c r="P9" s="3"/>
       <c r="Q9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R9" s="2">
         <v>8.6697999999999997E-2</v>
       </c>
-      <c r="S9" s="9"/>
+      <c r="S9" s="3"/>
       <c r="T9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="U9" s="12">
+      <c r="U9" s="5">
         <v>8.7001999999999996E-2</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="10">
         <v>8.3187999999999998E-2</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2">
         <v>8.2891000000000006E-2</v>
       </c>
-      <c r="G10" s="9"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="2">
         <v>8.4576999999999999E-2</v>
       </c>
-      <c r="J10" s="9"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L10" s="2">
         <v>8.2964999999999997E-2</v>
       </c>
-      <c r="M10" s="9"/>
+      <c r="M10" s="3"/>
       <c r="N10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="O10" s="2">
         <v>8.3490999999999996E-2</v>
       </c>
-      <c r="P10" s="9"/>
+      <c r="P10" s="3"/>
       <c r="Q10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="R10" s="2">
         <v>8.3571999999999994E-2</v>
       </c>
-      <c r="S10" s="9"/>
+      <c r="S10" s="3"/>
       <c r="T10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="U10" s="12">
+      <c r="U10" s="5">
         <v>8.2358000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="10">
         <v>8.2117999999999997E-2</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="2">
         <v>8.2624000000000003E-2</v>
       </c>
-      <c r="G11" s="9"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="2">
         <v>8.3276000000000003E-2</v>
       </c>
-      <c r="J11" s="9"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L11" s="2">
         <v>8.2603999999999997E-2</v>
       </c>
-      <c r="M11" s="9"/>
+      <c r="M11" s="3"/>
       <c r="N11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="O11" s="2">
         <v>8.3089999999999997E-2</v>
       </c>
-      <c r="P11" s="9"/>
+      <c r="P11" s="3"/>
       <c r="Q11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="R11" s="2">
         <v>8.2483000000000001E-2</v>
       </c>
-      <c r="S11" s="9"/>
+      <c r="S11" s="3"/>
       <c r="T11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U11" s="12">
+      <c r="U11" s="5">
         <v>7.9996999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="10">
         <v>8.1433000000000005E-2</v>
       </c>
-      <c r="D12" s="9"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="2">
         <v>8.2106999999999999E-2</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I12" s="2">
         <v>8.0867999999999995E-2</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L12" s="2">
         <v>7.9950999999999994E-2</v>
       </c>
-      <c r="M12" s="9"/>
+      <c r="M12" s="3"/>
       <c r="N12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O12" s="2">
         <v>8.2350000000000007E-2</v>
       </c>
-      <c r="P12" s="9"/>
+      <c r="P12" s="3"/>
       <c r="Q12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="R12" s="2">
         <v>8.1570000000000004E-2</v>
       </c>
-      <c r="S12" s="9"/>
+      <c r="S12" s="3"/>
       <c r="T12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U12" s="12">
+      <c r="U12" s="5">
         <v>7.9957E-2</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="10">
         <v>7.4489E-2</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="2">
         <v>7.4403999999999998E-2</v>
       </c>
-      <c r="G13" s="9"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="2">
         <v>7.3608000000000007E-2</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="L13" s="2">
         <v>7.3536000000000004E-2</v>
       </c>
-      <c r="M13" s="9"/>
+      <c r="M13" s="3"/>
       <c r="N13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="O13" s="2">
         <v>7.2997000000000006E-2</v>
       </c>
-      <c r="P13" s="9"/>
+      <c r="P13" s="3"/>
       <c r="Q13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R13" s="2">
         <v>7.3927000000000007E-2</v>
       </c>
-      <c r="S13" s="9"/>
+      <c r="S13" s="3"/>
       <c r="T13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="U13" s="12">
+      <c r="U13" s="5">
         <v>7.3509000000000005E-2</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="10">
         <v>6.5318000000000001E-2</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="2">
         <v>6.6005999999999995E-2</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I14" s="2">
         <v>6.7002000000000006E-2</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L14" s="2">
         <v>6.7198999999999995E-2</v>
       </c>
-      <c r="M14" s="9"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="O14" s="2">
         <v>6.5891000000000005E-2</v>
       </c>
-      <c r="P14" s="9"/>
+      <c r="P14" s="3"/>
       <c r="Q14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R14" s="2">
         <v>6.6286999999999999E-2</v>
       </c>
-      <c r="S14" s="9"/>
+      <c r="S14" s="3"/>
       <c r="T14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="U14" s="12">
+      <c r="U14" s="5">
         <v>6.6604999999999998E-2</v>
       </c>
     </row>
     <row r="15" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="12">
         <v>6.3576999999999995E-2</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="7">
         <v>6.3654000000000002E-2</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="14" t="s">
+      <c r="G15" s="8"/>
+      <c r="H15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="7">
         <v>6.4124E-2</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="14" t="s">
+      <c r="J15" s="8"/>
+      <c r="K15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="7">
         <v>6.3281000000000004E-2</v>
       </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="14" t="s">
+      <c r="M15" s="8"/>
+      <c r="N15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O15" s="14">
+      <c r="O15" s="7">
         <v>6.4708000000000002E-2</v>
       </c>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="14" t="s">
+      <c r="P15" s="8"/>
+      <c r="Q15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="R15" s="14">
+      <c r="R15" s="7">
         <v>6.5837000000000007E-2</v>
       </c>
-      <c r="S15" s="15"/>
-      <c r="T15" s="14" t="s">
+      <c r="S15" s="8"/>
+      <c r="T15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="16">
+      <c r="U15" s="9">
         <v>6.4905000000000004E-2</v>
       </c>
     </row>
     <row r="17" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="7"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="17"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="3" t="s">
+      <c r="C19" s="19"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="3" t="s">
+      <c r="F19" s="19"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="3" t="s">
+      <c r="I19" s="19"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="4"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="3" t="s">
+      <c r="L19" s="19"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="O19" s="4"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="3" t="s">
+      <c r="O19" s="19"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="R19" s="4"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="17" t="s">
+      <c r="R19" s="19"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="U19" s="18"/>
+      <c r="U19" s="22"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="9"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="9"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="9"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="L20" s="2"/>
-      <c r="M20" s="9"/>
+      <c r="M20" s="3"/>
       <c r="N20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O20" s="2"/>
-      <c r="P20" s="9"/>
+      <c r="P20" s="3"/>
       <c r="Q20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="R20" s="2"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="19" t="s">
+      <c r="S20" s="3"/>
+      <c r="T20" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="U20" s="20"/>
+      <c r="U20" s="11"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="2">
         <v>0.184973</v>
       </c>
-      <c r="D21" s="9"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F21" s="2">
         <v>0.184116</v>
       </c>
-      <c r="G21" s="9"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I21" s="2">
         <v>0.18201300000000001</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J21" s="3"/>
       <c r="K21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="L21" s="2">
         <v>0.18359800000000001</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M21" s="3"/>
       <c r="N21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="O21" s="2">
         <v>0.18770800000000001</v>
       </c>
-      <c r="P21" s="9"/>
+      <c r="P21" s="3"/>
       <c r="Q21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="R21" s="2">
         <v>0.16916900000000001</v>
       </c>
-      <c r="S21" s="9"/>
-      <c r="T21" s="19" t="s">
+      <c r="S21" s="3"/>
+      <c r="T21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="U21" s="20">
+      <c r="U21" s="11">
         <v>0.19017200000000001</v>
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="2">
         <v>0.129805</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="2">
         <v>0.128359</v>
       </c>
-      <c r="G22" s="9"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I22" s="2">
         <v>0.13082299999999999</v>
       </c>
-      <c r="J22" s="9"/>
+      <c r="J22" s="3"/>
       <c r="K22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L22" s="2">
         <v>0.133742</v>
       </c>
-      <c r="M22" s="9"/>
+      <c r="M22" s="3"/>
       <c r="N22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="O22" s="2">
         <v>0.123639</v>
       </c>
-      <c r="P22" s="9"/>
+      <c r="P22" s="3"/>
       <c r="Q22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="R22" s="2">
         <v>0.128853</v>
       </c>
-      <c r="S22" s="9"/>
-      <c r="T22" s="19" t="s">
+      <c r="S22" s="3"/>
+      <c r="T22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="U22" s="20">
+      <c r="U22" s="11">
         <v>0.13022700000000001</v>
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="2">
         <v>0.111883</v>
       </c>
-      <c r="D23" s="9"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F23" s="2">
         <v>0.11376</v>
       </c>
-      <c r="G23" s="9"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I23" s="2">
         <v>0.11040999999999999</v>
       </c>
-      <c r="J23" s="9"/>
+      <c r="J23" s="3"/>
       <c r="K23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L23" s="2">
         <v>0.10849300000000001</v>
       </c>
-      <c r="M23" s="9"/>
+      <c r="M23" s="3"/>
       <c r="N23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="O23" s="2">
         <v>0.113981</v>
       </c>
-      <c r="P23" s="9"/>
+      <c r="P23" s="3"/>
       <c r="Q23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="R23" s="2">
         <v>0.114429</v>
       </c>
-      <c r="S23" s="9"/>
-      <c r="T23" s="19" t="s">
+      <c r="S23" s="3"/>
+      <c r="T23" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="U23" s="20">
+      <c r="U23" s="11">
         <v>0.109526</v>
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="2">
         <v>9.8177E-2</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="2">
         <v>9.9115999999999996E-2</v>
       </c>
-      <c r="G24" s="9"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I24" s="2">
         <v>0.103654</v>
       </c>
-      <c r="J24" s="9"/>
+      <c r="J24" s="3"/>
       <c r="K24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L24" s="2">
         <v>9.9914000000000003E-2</v>
       </c>
-      <c r="M24" s="9"/>
+      <c r="M24" s="3"/>
       <c r="N24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="O24" s="2">
         <v>9.9728999999999998E-2</v>
       </c>
-      <c r="P24" s="9"/>
+      <c r="P24" s="3"/>
       <c r="Q24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R24" s="2">
         <v>0.10395</v>
       </c>
-      <c r="S24" s="9"/>
-      <c r="T24" s="19" t="s">
+      <c r="S24" s="3"/>
+      <c r="T24" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="U24" s="20">
+      <c r="U24" s="11">
         <v>9.9821999999999994E-2</v>
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="2">
         <v>8.5746000000000003E-2</v>
       </c>
-      <c r="D25" s="9"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F25" s="2">
         <v>8.9677000000000007E-2</v>
       </c>
-      <c r="G25" s="9"/>
+      <c r="G25" s="3"/>
       <c r="H25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I25" s="2">
         <v>8.6901999999999993E-2</v>
       </c>
-      <c r="J25" s="9"/>
+      <c r="J25" s="3"/>
       <c r="K25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L25" s="2">
         <v>9.0342000000000006E-2</v>
       </c>
-      <c r="M25" s="9"/>
+      <c r="M25" s="3"/>
       <c r="N25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="O25" s="2">
         <v>8.8405999999999998E-2</v>
       </c>
-      <c r="P25" s="9"/>
+      <c r="P25" s="3"/>
       <c r="Q25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="R25" s="2">
         <v>9.3692999999999999E-2</v>
       </c>
-      <c r="S25" s="9"/>
-      <c r="T25" s="19" t="s">
+      <c r="S25" s="3"/>
+      <c r="T25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="U25" s="20">
+      <c r="U25" s="11">
         <v>8.7103E-2</v>
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="2">
         <v>7.4959999999999999E-2</v>
       </c>
-      <c r="D26" s="9"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F26" s="2">
         <v>7.3994000000000004E-2</v>
       </c>
-      <c r="G26" s="9"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I26" s="2">
         <v>7.4253E-2</v>
       </c>
-      <c r="J26" s="9"/>
+      <c r="J26" s="3"/>
       <c r="K26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L26" s="2">
         <v>7.3802000000000006E-2</v>
       </c>
-      <c r="M26" s="9"/>
+      <c r="M26" s="3"/>
       <c r="N26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="O26" s="2">
         <v>7.2777999999999995E-2</v>
       </c>
-      <c r="P26" s="9"/>
+      <c r="P26" s="3"/>
       <c r="Q26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="R26" s="2">
         <v>7.3979000000000003E-2</v>
       </c>
-      <c r="S26" s="9"/>
-      <c r="T26" s="19" t="s">
+      <c r="S26" s="3"/>
+      <c r="T26" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="U26" s="20">
+      <c r="U26" s="11">
         <v>7.2655999999999998E-2</v>
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="2">
         <v>7.0065000000000002E-2</v>
       </c>
-      <c r="D27" s="9"/>
+      <c r="D27" s="3"/>
       <c r="E27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="2">
         <v>6.7590999999999998E-2</v>
       </c>
-      <c r="G27" s="9"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I27" s="2">
         <v>6.6291000000000003E-2</v>
       </c>
-      <c r="J27" s="9"/>
+      <c r="J27" s="3"/>
       <c r="K27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L27" s="2">
         <v>6.6142000000000006E-2</v>
       </c>
-      <c r="M27" s="9"/>
+      <c r="M27" s="3"/>
       <c r="N27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="O27" s="2">
         <v>6.8940000000000001E-2</v>
       </c>
-      <c r="P27" s="9"/>
+      <c r="P27" s="3"/>
       <c r="Q27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R27" s="2">
         <v>6.9912000000000002E-2</v>
       </c>
-      <c r="S27" s="9"/>
-      <c r="T27" s="19" t="s">
+      <c r="S27" s="3"/>
+      <c r="T27" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="U27" s="20">
+      <c r="U27" s="11">
         <v>6.7912E-2</v>
       </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="2">
         <v>6.6845000000000002E-2</v>
       </c>
-      <c r="D28" s="9"/>
+      <c r="D28" s="3"/>
       <c r="E28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="2">
         <v>6.5676999999999999E-2</v>
       </c>
-      <c r="G28" s="9"/>
+      <c r="G28" s="3"/>
       <c r="H28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I28" s="2">
         <v>6.5895999999999996E-2</v>
       </c>
-      <c r="J28" s="9"/>
+      <c r="J28" s="3"/>
       <c r="K28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="L28" s="2">
         <v>6.5623000000000001E-2</v>
       </c>
-      <c r="M28" s="9"/>
+      <c r="M28" s="3"/>
       <c r="N28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="O28" s="2">
         <v>6.6840999999999998E-2</v>
       </c>
-      <c r="P28" s="9"/>
+      <c r="P28" s="3"/>
       <c r="Q28" s="2" t="s">
         <v>10</v>
       </c>
       <c r="R28" s="2">
         <v>6.4782000000000006E-2</v>
       </c>
-      <c r="S28" s="9"/>
-      <c r="T28" s="19" t="s">
+      <c r="S28" s="3"/>
+      <c r="T28" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="U28" s="20">
+      <c r="U28" s="11">
         <v>6.5842999999999999E-2</v>
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="2">
         <v>6.1052000000000002E-2</v>
       </c>
-      <c r="D29" s="9"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="2">
         <v>6.3969999999999999E-2</v>
       </c>
-      <c r="G29" s="9"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I29" s="2">
         <v>6.5158999999999995E-2</v>
       </c>
-      <c r="J29" s="9"/>
+      <c r="J29" s="3"/>
       <c r="K29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L29" s="2">
         <v>6.4876000000000003E-2</v>
       </c>
-      <c r="M29" s="9"/>
+      <c r="M29" s="3"/>
       <c r="N29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O29" s="2">
         <v>6.3481999999999997E-2</v>
       </c>
-      <c r="P29" s="9"/>
+      <c r="P29" s="3"/>
       <c r="Q29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="R29" s="2">
         <v>6.4449999999999993E-2</v>
       </c>
-      <c r="S29" s="9"/>
-      <c r="T29" s="19" t="s">
+      <c r="S29" s="3"/>
+      <c r="T29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="U29" s="20">
+      <c r="U29" s="11">
         <v>6.3453999999999997E-2</v>
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="2">
         <v>6.0358000000000002E-2</v>
       </c>
-      <c r="D30" s="9"/>
+      <c r="D30" s="3"/>
       <c r="E30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F30" s="2">
         <v>5.8444000000000003E-2</v>
       </c>
-      <c r="G30" s="9"/>
+      <c r="G30" s="3"/>
       <c r="H30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I30" s="2">
         <v>5.8283000000000001E-2</v>
       </c>
-      <c r="J30" s="9"/>
+      <c r="J30" s="3"/>
       <c r="K30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L30" s="2">
         <v>5.6763000000000001E-2</v>
       </c>
-      <c r="M30" s="9"/>
+      <c r="M30" s="3"/>
       <c r="N30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="O30" s="2">
         <v>5.7764999999999997E-2</v>
       </c>
-      <c r="P30" s="9"/>
+      <c r="P30" s="3"/>
       <c r="Q30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="R30" s="2">
         <v>5.8930000000000003E-2</v>
       </c>
-      <c r="S30" s="9"/>
-      <c r="T30" s="19" t="s">
+      <c r="S30" s="3"/>
+      <c r="T30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="U30" s="20">
+      <c r="U30" s="11">
         <v>5.8382999999999997E-2</v>
       </c>
     </row>
     <row r="31" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="7">
         <v>5.6136999999999999E-2</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="14" t="s">
+      <c r="D31" s="8"/>
+      <c r="E31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="7">
         <v>5.5295999999999998E-2</v>
       </c>
-      <c r="G31" s="15"/>
-      <c r="H31" s="14" t="s">
+      <c r="G31" s="8"/>
+      <c r="H31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="14">
+      <c r="I31" s="7">
         <v>5.6316999999999999E-2</v>
       </c>
-      <c r="J31" s="15"/>
-      <c r="K31" s="14" t="s">
+      <c r="J31" s="8"/>
+      <c r="K31" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L31" s="14">
+      <c r="L31" s="7">
         <v>5.6705999999999999E-2</v>
       </c>
-      <c r="M31" s="15"/>
-      <c r="N31" s="14" t="s">
+      <c r="M31" s="8"/>
+      <c r="N31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O31" s="14">
+      <c r="O31" s="7">
         <v>5.6730999999999997E-2</v>
       </c>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="14" t="s">
+      <c r="P31" s="8"/>
+      <c r="Q31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="R31" s="14">
+      <c r="R31" s="7">
         <v>5.7854000000000003E-2</v>
       </c>
-      <c r="S31" s="15"/>
-      <c r="T31" s="21" t="s">
+      <c r="S31" s="8"/>
+      <c r="T31" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="U31" s="22">
+      <c r="U31" s="13">
         <v>5.4901999999999999E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B2:U2"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="B18:U18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="E19:F19"/>
@@ -2118,14 +2134,6 @@
     <mergeCell ref="N19:O19"/>
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="T19:U19"/>
-    <mergeCell ref="B2:U2"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2137,7 +2145,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2145,7 +2153,7 @@
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="11.44140625" customWidth="1"/>
-    <col min="8" max="8" width="38.77734375" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.77734375" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="11.44140625" customWidth="1"/>
@@ -2173,7 +2181,7 @@
       <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="14" t="s">
         <v>28</v>
       </c>
       <c r="I1" t="s">
@@ -2205,7 +2213,7 @@
       <c r="F2">
         <v>0.74</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="14" t="s">
         <v>34</v>
       </c>
       <c r="J2">
@@ -2231,7 +2239,7 @@
       <c r="F3">
         <v>0.75</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="14" t="s">
         <v>34</v>
       </c>
       <c r="J3">
@@ -2254,20 +2262,56 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="F6">
+        <v>0.74</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0.79110000000000003</v>
+      </c>
+      <c r="F7">
+        <v>0.79</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
@@ -2289,7 +2333,7 @@
       <c r="F8">
         <v>0.78</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="14" t="s">
         <v>46</v>
       </c>
       <c r="J8">
@@ -2315,7 +2359,7 @@
       <c r="F9">
         <v>0.82</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="14" t="s">
         <v>48</v>
       </c>
       <c r="J9">

</xml_diff>

<commit_message>
Updates RF models, saves trees
</commit_message>
<xml_diff>
--- a/Model Results Overview.xlsx
+++ b/Model Results Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df8978671778c259/Desktop/repos/Homework/Wine_Quality_Predictor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{C5952579-04A8-4BFA-A758-230286535F9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5943BEF4-6DED-476F-B908-C9EF8D2191D8}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="8_{C5952579-04A8-4BFA-A758-230286535F9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4F619918-6690-4237-A9F2-7B49F665D277}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8A3C5073-7F06-4D4F-B578-7570066F7EA9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="62">
   <si>
     <t>Power transformer</t>
   </si>
@@ -130,9 +130,6 @@
     <t>random_state</t>
   </si>
   <si>
-    <t>max_iter</t>
-  </si>
-  <si>
     <t>Jeni</t>
   </si>
   <si>
@@ -145,15 +142,7 @@
     <t>Standard</t>
   </si>
   <si>
-    <t>Top 5 features used: Alcohol, sulphates, volatile acidity, total sulfur dioxide, density
-Per Grid Search best params;criterion= 'gini', max_depth= 125, n_estimators=50</t>
-  </si>
-  <si>
     <t>Power Transformer</t>
-  </si>
-  <si>
-    <t>Top 5 features: Alcohol, volatile acidity, density, free sulfur dioxide, total sulfur dioxide
-Per GridSearch best params: 'criterion': 'gini', 'max_depth': 125, 'n_estimators': 50</t>
   </si>
   <si>
     <t>Top Features: Alcohol, sulphates. Free sulfur dioxide, chlorides, volatile acidity, total sulfure dioxide
@@ -200,6 +189,57 @@
     <t xml:space="preserve">
 Top features only excluded residual sugar and chlorides
 best params: activation= 'relu', hidden_layer_sizes= (100, 2), learning_rate='constant'</t>
+  </si>
+  <si>
+    <t>Pros of Model</t>
+  </si>
+  <si>
+    <t>Cons of Model</t>
+  </si>
+  <si>
+    <t>*not good with skewed features
+* not good with data that has many outliers</t>
+  </si>
+  <si>
+    <t>* Good for binary target variable
+*good for smaller datasets(like ours)
+*good for determining feature importance
+* good baseline model</t>
+  </si>
+  <si>
+    <t>* good for classiication problem with binary target
+* handles outliers well</t>
+  </si>
+  <si>
+    <t>* hard to get feature importance, longer to train</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- good for categorical and continuous target variable
+-handles complex data</t>
+  </si>
+  <si>
+    <t>* hard to get feature importance- slower model</t>
+  </si>
+  <si>
+    <t>- good for categorical and continuous target varaibles
+good quick benchmark model</t>
+  </si>
+  <si>
+    <t>- not good for complex problems
+- does not show details within model
+- model does not learn from other trees within model</t>
+  </si>
+  <si>
+    <t>model may be too complex for our data set</t>
+  </si>
+  <si>
+    <t>Top 5 features used: Alcohol, sulphates, volatile acidity, total sulfur dioxide, density
+Per Grid Search best params;criterion= 'entropy', max_depth= 300, n_estimators=100</t>
+  </si>
+  <si>
+    <t>Top 5 features: Alcohol, volatile acidity, density, free sulfur dioxide, total sulfur dioxide
+Per GridSearch best params: 'criterion': 'entropy 'max_depth': 175, 'n_estimators': 250</t>
   </si>
 </sst>
 </file>
@@ -223,7 +263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,8 +282,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -433,11 +479,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -464,26 +536,52 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -859,37 +957,37 @@
       <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="19"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="19"/>
+      <c r="I3" s="20"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="19"/>
+      <c r="L3" s="20"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="19"/>
+      <c r="O3" s="20"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="19"/>
+      <c r="R3" s="20"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="20" t="s">
+      <c r="T3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="23"/>
+      <c r="U3" s="19"/>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
@@ -1503,40 +1601,40 @@
       <c r="U18" s="17"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="19"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="19"/>
+      <c r="I19" s="20"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="20" t="s">
+      <c r="K19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="19"/>
+      <c r="L19" s="20"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="20" t="s">
+      <c r="N19" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="O19" s="19"/>
+      <c r="O19" s="20"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="20" t="s">
+      <c r="Q19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="R19" s="19"/>
+      <c r="R19" s="20"/>
       <c r="S19" s="3"/>
       <c r="T19" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="U19" s="22"/>
+      <c r="U19" s="24"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
@@ -2126,6 +2224,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B18:U18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="T19:U19"/>
     <mergeCell ref="B2:U2"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="Q3:R3"/>
@@ -2134,14 +2240,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B18:U18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="T19:U19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2150,352 +2248,430 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7D50C4-F0EC-46BD-A61A-8BDA32A6521F}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="11.44140625" customWidth="1"/>
     <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.44140625" customWidth="1"/>
-    <col min="9" max="9" width="38.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="59.44140625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="28.33203125" style="32" customWidth="1"/>
+    <col min="13" max="13" width="27.5546875" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="27">
+        <v>0.746</v>
+      </c>
+      <c r="F2" s="27">
+        <v>0.74</v>
+      </c>
+      <c r="G2" s="27">
+        <v>0.74</v>
+      </c>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27">
+        <v>42</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="27">
+        <v>0.754</v>
+      </c>
+      <c r="F3" s="27">
+        <v>0.745</v>
+      </c>
+      <c r="G3" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27">
+        <v>42</v>
+      </c>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+    </row>
+    <row r="4" spans="1:14" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="D4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="27">
+        <v>0.749</v>
+      </c>
+      <c r="F4" s="27">
+        <v>0.73</v>
+      </c>
+      <c r="G4" s="27">
+        <v>0.73</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27">
+        <v>42</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B5" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E5" s="27">
+        <v>0.754</v>
+      </c>
+      <c r="F5" s="27">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="G5" s="27">
+        <v>0.74</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27">
+        <v>42</v>
+      </c>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+    </row>
+    <row r="6" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="27">
+        <v>1</v>
+      </c>
+      <c r="F6" s="27">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0.74</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27">
+        <v>42</v>
+      </c>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+    </row>
+    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="27">
+        <v>1</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0.79110000000000003</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0.79</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27">
+        <v>42</v>
+      </c>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+    </row>
+    <row r="8" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2">
-        <v>0.746</v>
-      </c>
-      <c r="F2">
-        <v>0.74</v>
-      </c>
-      <c r="G2">
-        <v>0.74</v>
-      </c>
-      <c r="I2" s="14" t="s">
+      <c r="D8" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="K2">
+      <c r="E8" s="27">
+        <v>1</v>
+      </c>
+      <c r="F8" s="27">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="G8" s="27">
+        <v>0.78</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="L8" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0.999</v>
+      </c>
+      <c r="F9" s="27">
+        <v>0.81869999999999998</v>
+      </c>
+      <c r="G9" s="27">
+        <v>0.82</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3">
-        <v>0.754</v>
-      </c>
-      <c r="F3">
-        <v>0.745</v>
-      </c>
-      <c r="G3">
-        <v>0.75</v>
-      </c>
-      <c r="I3" s="14" t="s">
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+    </row>
+    <row r="10" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="K3">
+      <c r="E10" s="27">
+        <v>0.81230000000000002</v>
+      </c>
+      <c r="F10" s="27">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="G10" s="27">
+        <v>0.78</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="L10" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4">
-        <v>0.749</v>
-      </c>
-      <c r="F4">
-        <v>0.73</v>
-      </c>
-      <c r="G4">
-        <v>0.73</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4">
+      <c r="D11" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0.83279999999999998</v>
+      </c>
+      <c r="F11" s="27">
+        <v>0.77629999999999999</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0.78</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5">
-        <v>0.754</v>
-      </c>
-      <c r="F5">
-        <v>0.74299999999999999</v>
-      </c>
-      <c r="G5">
-        <v>0.74</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0.74375000000000002</v>
-      </c>
-      <c r="G6">
-        <v>0.74</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0.79110000000000003</v>
-      </c>
-      <c r="G7">
-        <v>0.79</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8">
-        <v>0.999</v>
-      </c>
-      <c r="F8">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="G8">
-        <v>0.78</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9">
-        <v>0.999</v>
-      </c>
-      <c r="F9">
-        <v>0.81630000000000003</v>
-      </c>
-      <c r="G9">
-        <v>0.82</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10">
-        <v>0.81230000000000002</v>
-      </c>
-      <c r="F10">
-        <v>0.77749999999999997</v>
-      </c>
-      <c r="G10">
-        <v>0.78</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="K10">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11">
-        <v>0.83279999999999998</v>
-      </c>
-      <c r="F11">
-        <v>0.77629999999999999</v>
-      </c>
-      <c r="G11">
-        <v>0.78</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11">
-        <v>42</v>
-      </c>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>